<commit_message>
Note added to carriages BOM
Clearance issue might occur between Nema14 motor and X cross Member.
Ref: https://github.com/MirageC79/HextrudORT/issues/9
</commit_message>
<xml_diff>
--- a/files/CARRIAGE/HD12/BOM_HextrudORT_Carriage_HD12.xlsx
+++ b/files/CARRIAGE/HD12/BOM_HextrudORT_Carriage_HD12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\CARRIAGE\HD12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C90872C-BBF7-4E7F-9941-C83969EC3704}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566511DC-2570-415D-9B49-FACA4D5F29EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -175,6 +175,76 @@
 For Bearing provided with BMG (MR85 5x8x2.5) use:
 HextrudORT_HD12_CarriageBAckPlate_Body.stl</t>
     </r>
+  </si>
+  <si>
+    <t>OPTION B: Bearing_MR85 (from BMG)</t>
+  </si>
+  <si>
+    <t>Bearing 5X8X2.5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OPTION B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Use MR85 5x8x2.5 bearings from BMG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OPTION A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+These are BIGGER bearings than the ones used in the BMG.
+ To be used with Back Plate and cover marked with "BB"</t>
+    </r>
+  </si>
+  <si>
+    <t>1*</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:4790412</t>
+  </si>
+  <si>
+    <t>Bearing, 9X5X3</t>
   </si>
   <si>
     <r>
@@ -206,29 +276,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>DO NOT SET CURRENT HIGHER THAN 0.400ma in your printer config file.
+      <t xml:space="preserve">DO NOT SET CURRENT HIGHER THAN 0.400ma in your printer config file.
 These motors are Class H and are rated for 180C, they can become VERY HOT and might melt your carriage
 Spec:
-https://miragec79.github.io/HextrudORT/docs/LDO-36STH17-1004AHG-RevA_1.pdf</t>
+https://miragec79.github.io/HextrudORT/docs/LDO-36STH17-1004AHG-RevA_1.pdf
+</t>
     </r>
-  </si>
-  <si>
-    <t>OPTION B: Bearing_MR85 (from BMG)</t>
-  </si>
-  <si>
-    <t>Bearing 5X8X2.5</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="3"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>OPTION B</t>
+      <t xml:space="preserve">Important Note: ref: https://github.com/MirageC79/HextrudORT/issues/9
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Depending on source of components, printing tolerances and the fact that the design clearances are reduced to a minimal, you may need to file/trim a section of the Nema 14 motor to clear the XY cross member.
+This modifcation will not affect motor performance or reliability.</t>
     </r>
     <r>
       <rPr>
@@ -239,48 +314,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Use MR85 5x8x2.5 bearings from BMG</t>
+</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OPTION A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-These are BIGGER bearings than the ones used in the BMG.
- To be used with Back Plate and cover marked with "BB"</t>
-    </r>
-  </si>
-  <si>
-    <t>1*</t>
-  </si>
-  <si>
-    <t>3a</t>
-  </si>
-  <si>
-    <t>3b</t>
-  </si>
-  <si>
-    <t>https://www.thingiverse.com/thing:4790412</t>
-  </si>
-  <si>
-    <t>Bearing, 9X5X3</t>
   </si>
 </sst>
 </file>
@@ -1694,24 +1729,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="9" max="9" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="71.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1746,7 +1781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="18" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
@@ -1766,12 +1801,12 @@
         <v>1</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1798,7 +1833,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="17"/>
     </row>
-    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>37</v>
       </c>
@@ -1825,7 +1860,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="17"/>
     </row>
-    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -1852,7 +1887,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="17"/>
     </row>
-    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
@@ -1879,7 +1914,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
@@ -1906,7 +1941,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
@@ -1933,7 +1968,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
@@ -1960,7 +1995,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
@@ -1987,7 +2022,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
@@ -2014,7 +2049,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
@@ -2041,11 +2076,11 @@
         <v>42</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>37</v>
       </c>
@@ -2072,7 +2107,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2134,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>37</v>
       </c>
@@ -2107,28 +2142,28 @@
         <v>39</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>44</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>45</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>39</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15" s="22"/>
       <c r="K15" s="26"/>
     </row>
-    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>37</v>
       </c>
@@ -2136,23 +2171,23 @@
         <v>39</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="17"/>
@@ -2160,12 +2195,13 @@
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <webPublishItems count="1">
     <webPublishItem id="27803" divId="BOM_HextrudORT_Carriage_HD12_27803" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\CARRIAGE\HD12\BOM_HextrudORT_Carriage_HD12.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected Thingiverse and GitHub links
</commit_message>
<xml_diff>
--- a/files/CARRIAGE/HD12/BOM_HextrudORT_Carriage_HD12.xlsx
+++ b/files/CARRIAGE/HD12/BOM_HextrudORT_Carriage_HD12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\CARRIAGE\HD12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566511DC-2570-415D-9B49-FACA4D5F29EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427665EA-C111-408A-96B9-B177A508F98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>3b</t>
-  </si>
-  <si>
-    <t>https://www.thingiverse.com/thing:4790412</t>
   </si>
   <si>
     <t>Bearing, 9X5X3</t>
@@ -316,6 +313,14 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>Thingiverse
+Alternate: GitHub</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:4790412
+alternate: https://github.com/MirageC79/HextrudORT/tree/main/files/CARRIAGE/HD12/STL</t>
   </si>
 </sst>
 </file>
@@ -580,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -656,6 +661,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1729,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1743,7 +1751,7 @@
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="9" max="9" width="71.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.81640625" customWidth="1"/>
-    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="11" max="11" width="41.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1801,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="17"/>
@@ -2075,10 +2083,12 @@
       <c r="I12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" s="17"/>
+      <c r="J12" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
@@ -2104,8 +2114,12 @@
         <v>1</v>
       </c>
       <c r="I13" s="16"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="17"/>
+      <c r="J13" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
@@ -2131,8 +2145,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="16"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="17"/>
+      <c r="J14" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
@@ -2178,7 +2196,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>12</v>

</xml_diff>